<commit_message>
Rerunning error extraction + results
</commit_message>
<xml_diff>
--- a/data/results/all_lemmas.xlsx
+++ b/data/results/all_lemmas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1002,3466 +1002,3466 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>519</v>
+        <v>544</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Chyrowskiey</t>
+          <t>Pierściorowskim</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Posadzie Chyrowskiey zapędziły</t>
+          <t>pierwszym Pierściorowskim miała</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>chyrowska</t>
+          <t>Pierściorowski</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Chyrowskiey</t>
+          <t>Pierściorowskim</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>chyrowski</t>
+          <t>pierściorowski</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pierściorowskim</t>
+          <t>Maryę</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pierwszym Pierściorowskim miała</t>
+          <t>córkę Maryę ,</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Pierściorowski</t>
+          <t>Marya</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Pierściorowskim</t>
+          <t>Maryę</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>pierściorowski</t>
+          <t>marya</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Maryę</t>
+          <t>Kleofasę</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>córkę Maryę ,</t>
+          <t>, Kleofasę .</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Marya</t>
+          <t>Kleofasa</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Maryę</t>
+          <t>Kleofasę</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>marya</t>
+          <t>kleofasa</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>549</v>
+        <v>606</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kleofasę</t>
+          <t>Asińdźka</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>, Kleofasę .</t>
+          <t>wiesz Asińdźka co</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Kleofasa</t>
+          <t>Asińdźka</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Kleofasę</t>
+          <t>asińdźka</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>kleofasa</t>
+          <t>asińdźka</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>606</v>
+        <v>648</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Asińdźka</t>
+          <t>Kleosię</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>wiesz Asińdźka co</t>
+          <t>moją Kleosię ”</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Asińdźka</t>
+          <t>Kleosia</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>asińdźka</t>
+          <t>Kleosię</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>asińdźka</t>
+          <t>kleosia</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>648</v>
+        <v>694</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Kleosię</t>
+          <t>Pannie</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>moją Kleosię ”</t>
+          <t>wstąpi Pannie się</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kleosia</t>
+          <t>panna</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Kleosię</t>
+          <t>Panna</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>kleosia</t>
+          <t>pani</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>694</v>
+        <v>729</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Pannie</t>
+          <t>Czołhanach</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>wstąpi Pannie się</t>
+          <t>w Czołhanach roku</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>panna</t>
+          <t>Czołhany</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Panna</t>
+          <t>Czołhanach</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>pani</t>
+          <t>czołhanin</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>729</v>
+        <v>739</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Czołhanach</t>
+          <t>osiedli</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>w Czołhanach roku</t>
+          <t>nauki osiedli na</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Czołhany</t>
+          <t>osiąść</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Czołhanach</t>
+          <t>osiedle</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>czołhanin</t>
+          <t>osiedle</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>739</v>
+        <v>756</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>osiedli</t>
+          <t>Bolechowie</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>nauki osiedli na</t>
+          <t>w Bolechowie umarła</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>osiąść</t>
+          <t>Bolechów</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>osiedle</t>
+          <t>Bolechowo</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>osiedle</t>
+          <t>bolech</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>756</v>
+        <v>784</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Bolechowie</t>
+          <t>Maksymowic</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>w Bolechowie umarła</t>
+          <t>właściciela Maksymowic w</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Bolechów</t>
+          <t>Maksymowice</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Bolechowo</t>
+          <t>Maksymowic</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>bolech</t>
+          <t>maksymowica</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Maksymowic</t>
+          <t>Stan</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>właściciela Maksymowic w</t>
+          <t>za Stan .</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Maksymowice</t>
+          <t>Stanisław</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Maksymowic</t>
+          <t>Stan</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>maksymowica</t>
+          <t>stan</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Stan</t>
+          <t>Aug</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>za Stan .</t>
+          <t>. Aug .</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Stanisława</t>
+          <t>August</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Stan</t>
+          <t>Aug</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>stan</t>
+          <t>aug</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>798</v>
+        <v>814</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Aug</t>
+          <t>Bludnikach</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>. Aug .</t>
+          <t>w Bludnikach –</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Augusta</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Aug</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>aug</t>
+          <t>Bludnik</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>814</v>
+        <v>852</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Bludnikach</t>
+          <t>bombardowaniu</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>w Bludnikach –</t>
+          <t>Przy bombardowaniu Lwowa</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>bombardowanie</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>bombardować</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>bombardować</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>852</v>
+        <v>863</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bombardowaniu</t>
+          <t>obrucona</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Przy bombardowaniu Lwowa</t>
+          <t>perzynę obrucona –</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>bombardowanie</t>
+          <t>obrucić</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>bombardować</t>
+          <t>obrucona</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>bombardować</t>
+          <t>obrucon</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>863</v>
+        <v>884</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>obrucona</t>
+          <t>niespotyka</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>perzynę obrucona –</t>
+          <t>się niespotyka .</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>obrucić</t>
+          <t>niespotykać</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>obrucona</t>
+          <t>niespotyka</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>obrucon</t>
+          <t>niespotyka</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>884</v>
+        <v>907</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>niespotyka</t>
+          <t>dobrami</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>się niespotyka .</t>
+          <t>wielkimi dobrami ,</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>niespotykać</t>
+          <t>dobra</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>niespotyka</t>
+          <t>dobro</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>niespotyka</t>
+          <t>dobro</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>907</v>
+        <v>934</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>dobrami</t>
+          <t>arye</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>wielkimi dobrami ,</t>
+          <t>różne arye krakowiaki</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>dobra</t>
+          <t>arya</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>dobro</t>
+          <t>arye</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>dobro</t>
+          <t>arye</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>934</v>
+        <v>1115</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>arye</t>
+          <t>Świerzawski</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>różne arye krakowiaki</t>
+          <t>wuj Świerzawski kuzyn</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>arya</t>
+          <t>Świerzawski</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>arye</t>
+          <t>świerzawski</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>arye</t>
+          <t>świerzawski</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Świerzawski</t>
+          <t>Polanowskich</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>wuj Świerzawski kuzyn</t>
+          <t>kuzyn Polanowskich z</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Świerzawski</t>
+          <t>Polanowski</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>świerzawski</t>
+          <t>polanowski</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>świerzawski</t>
+          <t>polanowski</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Polanowskich</t>
+          <t>Bełzkiego</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>kuzyn Polanowskich z</t>
+          <t>z Bełzkiego często</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Polanowski</t>
+          <t>Bełzkie</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>polanowski</t>
+          <t>Bełzkiego</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>polanowski</t>
+          <t>bełziek</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Bełzkiego</t>
+          <t>Moszkowie</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>z Bełzkiego często</t>
+          <t>w Moszkowie z</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Bełzkie</t>
+          <t>Moszków</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Bełzkiego</t>
+          <t>Moszek</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>bełziek</t>
+          <t>moszków</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>1123</v>
+        <v>1181</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Moszkowie</t>
+          <t>niepomięła</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>w Moszkowie z</t>
+          <t>Komornikowej niepomięła –</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Moszków</t>
+          <t>niepomiąć</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Moszek</t>
+          <t>niepomięła</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>moszków</t>
+          <t>niepomięło</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>1181</v>
+        <v>1215</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>niepomięła</t>
+          <t>Treterówną</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Komornikowej niepomięła –</t>
+          <t>siostrą Treterówną -</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>niepomiąć</t>
+          <t>Treterówna</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>niepomięła</t>
+          <t>Treterówną</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>niepomięło</t>
+          <t>treterówna</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1215</v>
+        <v>1233</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Treterówną</t>
+          <t>Rosyi</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>siostrą Treterówną -</t>
+          <t>w Rosyi –</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Treterówna</t>
+          <t>Rosya</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Treterówną</t>
+          <t>Rosyi</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>treterówna</t>
+          <t>rosej</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1233</v>
+        <v>1321</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Rosyi</t>
+          <t>ś</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>w Rosyi –</t>
+          <t>mi ś .</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Rosya</t>
+          <t>świętej</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Rosyi</t>
+          <t>ś</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>rosej</t>
+          <t>być</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1295</v>
+        <v>1323</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cobary</t>
+          <t>p</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sachsen Cobary Ułanów</t>
+          <t>. p .</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>cobary</t>
+          <t>pamięci</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Cobary</t>
+          <t>List_świętego_Piotra</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>cobar</t>
+          <t>pan</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>1321</v>
+        <v>1329</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ś</t>
+          <t>nieśmiał</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>mi ś .</t>
+          <t>ja nieśmiał em</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>świętej</t>
+          <t>nieśmieć</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ś</t>
+          <t>MISPARSED</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>być</t>
+          <t>nieśmiał</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1323</v>
+        <v>1334</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>niebył</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>. p .</t>
+          <t>Wreszcie niebył em</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>pamięci</t>
+          <t>niebyć</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>List_świętego_Piotra</t>
+          <t>MISPARSED</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>pan</t>
+          <t>niebył</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1329</v>
+        <v>1340</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>nieśmiał</t>
+          <t>Oycem</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ja nieśmiał em</t>
+          <t>z Oycem na</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>nieśmieć</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>MISPARSED</t>
+          <t>Oycem</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>nieśmiał</t>
+          <t>oycie</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>1334</v>
+        <v>1418</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>niebył</t>
+          <t>kończ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Wreszcie niebył em</t>
+          <t>do kończ życia</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>niebyć</t>
+          <t>koniec</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>MISPARSED</t>
+          <t>kończyć</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>niebył</t>
+          <t>kończ</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>1340</v>
+        <v>1439</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Oycem</t>
+          <t>assekuracyi</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>z Oycem na</t>
+          <t>w assekuracyi armat</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>oyciec</t>
+          <t>assekuracya</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oycem</t>
+          <t>assekuracyi</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>oycie</t>
+          <t>assekuracyj</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>1418</v>
+        <v>1497</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>kończ</t>
+          <t>skrzętnem</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>do kończ życia</t>
+          <t>fortuny skrzętnem gospodarstwem</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>koniec</t>
+          <t>skrzętny</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>kończyć</t>
+          <t>skrzętnem</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>kończ</t>
+          <t>skrzętno</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>1439</v>
+        <v>1509</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>assekuracyi</t>
+          <t>tem</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>w assekuracyi armat</t>
+          <t>po tem jak</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>assekuracya</t>
+          <t>to</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>assekuracyi</t>
+          <t>tema</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>assekuracyj</t>
+          <t>tem</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>1497</v>
+        <v>1517</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>skrzętnem</t>
+          <t>set</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>fortuny skrzętnem gospodarstwem</t>
+          <t>parę set sztuk</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>skrzętny</t>
+          <t>sto</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>skrzętnem</t>
+          <t>seta</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>skrzętno</t>
+          <t>set</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1509</v>
+        <v>1527</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>tem</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>po tem jak</t>
+          <t>kupił Bludniki za</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>to</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>tema</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>tem</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>1517</v>
+        <v>1604</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>set</t>
+          <t>któremi</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>parę set sztuk</t>
+          <t>nad któremi obeymował</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>sto</t>
+          <t>który</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>seta</t>
+          <t>któremi</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>set</t>
+          <t>któr</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>1527</v>
+        <v>1605</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>obeymował</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>kupił Bludniki za</t>
+          <t>któremi obeymował Dziedzictwo</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>obeymować</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>obeymował</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>obeymował</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>1604</v>
+        <v>1609</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>któremi</t>
+          <t>juryzdyksye</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>nad któremi obeymował</t>
+          <t>prawną juryzdyksye sądową</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>który</t>
+          <t>juryzdyksya</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>któremi</t>
+          <t>juryzdyksye</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>któr</t>
+          <t>juryzdyksye</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>1605</v>
+        <v>1614</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>obeymował</t>
+          <t>pierwszey</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>któremi obeymował Dziedzictwo</t>
+          <t>policyjną pierwszey instantacyi</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>obeymować</t>
+          <t>pierwsza</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>obeymował</t>
+          <t>pierwszey</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>obeymował</t>
+          <t>pierwsze</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1609</v>
+        <v>1615</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>juryzdyksye</t>
+          <t>instantacyi</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>prawną juryzdyksye sądową</t>
+          <t>pierwszey instantacyi .</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>juryzdyksya</t>
+          <t>instantacya</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>juryzdyksye</t>
+          <t>instantacyi</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>juryzdyksye</t>
+          <t>instantaka</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>1614</v>
+        <v>1626</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>pierwszey</t>
+          <t>morgów</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>policyjną pierwszey instantacyi</t>
+          <t>posiadanych morgów -</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>pierwsza</t>
+          <t>morg</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>pierwszey</t>
+          <t>mórg</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>pierwsze</t>
+          <t>morge</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>1615</v>
+        <v>1734</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>instantacyi</t>
+          <t>Ostaszewskigo</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>pierwszey instantacyi .</t>
+          <t>Dziadka Ostaszewskigo jak</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>instantacya</t>
+          <t>Ostaszewski</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>instantacyi</t>
+          <t>Ostaszewskigo</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>instantaka</t>
+          <t>ostaszewski</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>1626</v>
+        <v>1741</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>morgów</t>
+          <t>kmiecie</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>posiadanych morgów -</t>
+          <t>jego kmiecie na</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>morg</t>
+          <t>kmieć</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>mórg</t>
+          <t>kmieci</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>morge</t>
+          <t>kmieta</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1693</v>
+        <v>1754</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>jaja</t>
+          <t>bydle</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>, jaja –</t>
+          <t>padło bydle robocze</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>jaja</t>
+          <t>bydlę</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>jaje</t>
+          <t>bydło</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>jajo</t>
+          <t>byska</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>1734</v>
+        <v>1772</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Ostaszewskigo</t>
+          <t>Dłużanie</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Dziadka Ostaszewskigo jak</t>
+          <t>raz Dłużanie żalili</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Ostaszewski</t>
+          <t>Dłużanin</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Ostaszewskigo</t>
+          <t>Dłużanie</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>ostaszewski</t>
+          <t>dłużać</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>1741</v>
+        <v>1777</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>kmiecie</t>
+          <t>niemają</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>jego kmiecie na</t>
+          <t>że niemają dogodnego</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>kmieć</t>
+          <t>niemieć</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>kmieci</t>
+          <t>niemaja</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>kmieta</t>
+          <t>niema</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>1754</v>
+        <v>1790</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>bydle</t>
+          <t>suchey</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>padło bydle robocze</t>
+          <t>morgów suchey łąki</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>bydlę</t>
+          <t>suchy</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>bydło</t>
+          <t>suchey</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>byska</t>
+          <t>suchey</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1772</v>
+        <v>1792</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Dłużanie</t>
+          <t>podedworem</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>raz Dłużanie żalili</t>
+          <t>łąki podedworem a</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Dłużanin</t>
+          <t>podedwór</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Dłużanie</t>
+          <t>podedworem</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>dłużać</t>
+          <t>podedwor</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>1777</v>
+        <v>1794</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>niemają</t>
+          <t>nayskładniey</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>że niemają dogodnego</t>
+          <t>a nayskładniey położone</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>niemieć</t>
+          <t>składnie</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>niemaja</t>
+          <t>nayskładniey</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>niema</t>
+          <t>nayskładnie</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>1790</v>
+        <v>1804</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>suchey</t>
+          <t>Niebył</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>morgów suchey łąki</t>
+          <t>. Niebył to</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>suchy</t>
+          <t>niebyć</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>suchey</t>
+          <t>Niebyła</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>suchey</t>
+          <t>niebył</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>1792</v>
+        <v>1830</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>podedworem</t>
+          <t>warżenia</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>łąki podedworem a</t>
+          <t>prawo warżenia piwa</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>podedwór</t>
+          <t>warżyć</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>podedworem</t>
+          <t>warżenia</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>podedwor</t>
+          <t>warżenie</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>1794</v>
+        <v>1881</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>nayskładniey</t>
+          <t>miarkmi</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>a nayskładniey położone</t>
+          <t>– miarkmi wianki</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>składnie</t>
+          <t>miarka</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>nayskładniey</t>
+          <t>miarkmi</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>nayskładnie</t>
+          <t>miarko</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>1804</v>
+        <v>1913</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Niebył</t>
+          <t>takiem</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>. Niebył to</t>
+          <t>przy takiem obciążeniu</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>niebyć</t>
+          <t>taki</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Niebyła</t>
+          <t>takiem</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>niebył</t>
+          <t>tak</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>1830</v>
+        <v>1938</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>warżenia</t>
+          <t>jurysdykcyi</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>prawo warżenia piwa</t>
+          <t>urzędowa jurysdykcyi był</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>warżyć</t>
+          <t>jurysdykcya</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>warżenia</t>
+          <t>jurysdykcyi</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>warżenie</t>
+          <t>jurysdykcyj</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>1881</v>
+        <v>1941</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>miarkmi</t>
+          <t>Dziedzica</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>– miarkmi wianki</t>
+          <t>Herb Dziedzica –</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>miarka</t>
+          <t>dziedzic</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>miarkmi</t>
+          <t>Dziedzic</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>miarko</t>
+          <t>dziedzica</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>1913</v>
+        <v>1947</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>takiem</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>przy takiem obciążeniu</t>
+          <t>Dominium Bludniki –</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>taki</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>takiem</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>tak</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>1938</v>
+        <v>1952</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>jurysdykcyi</t>
+          <t>t</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>urzędowa jurysdykcyi był</t>
+          <t>i t .</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>jurysdykcya</t>
+          <t>tym</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>jurysdykcyi</t>
+          <t>tona</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>jurysdykcyj</t>
+          <t>t</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>1941</v>
+        <v>1954</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Dziedzica</t>
+          <t>p</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Herb Dziedzica –</t>
+          <t>. p .</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>dziedzic</t>
+          <t>podobne</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Dziedzic</t>
+          <t>List_świętego_Piotra</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>dziedzica</t>
+          <t>pan</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>1947</v>
+        <v>1957</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>niemógł</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Dominium Bludniki –</t>
+          <t>Nieszlachcic niemógł kupować</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>niemóc</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>niemógł</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>niemógł</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>1952</v>
+        <v>1966</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>mieycus</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>i t .</t>
+          <t>swojem mieycus Mandatariusza</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>tym</t>
+          <t>mieysce</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>tona</t>
+          <t>mieycus</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>mieycus</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>1954</v>
+        <v>1997</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>niemogło</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>. p .</t>
+          <t>– niemogło się</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>podobne</t>
+          <t>niemóc</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>List_świętego_Piotra</t>
+          <t>niemogło</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>pan</t>
+          <t>niemogło</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>1957</v>
+        <v>2013</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>niemógł</t>
+          <t>nieprzyniósł</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Nieszlachcic niemógł kupować</t>
+          <t>Dominii nieprzyniósł kartki</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>niemóc</t>
+          <t>nieprzynieść</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>niemógł</t>
+          <t>nieprzyniósł</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>niemógł</t>
+          <t>nieprzyniósło</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>1966</v>
+        <v>2121</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>mieycus</t>
+          <t>ludowemi</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>swojem mieycus Mandatariusza</t>
+          <t>dziś ludowemi zwanych</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>mieysce</t>
+          <t>ludowe</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>mieycus</t>
+          <t>ludowemi</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>mieycus</t>
+          <t>ludowa</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>1997</v>
+        <v>2149</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>niemogło</t>
+          <t>manipulacyi</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>– niemogło się</t>
+          <t>– manipulacyi urzędowey</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>niemóc</t>
+          <t>manipulacya</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>niemogło</t>
+          <t>manipulacyi</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>niemogło</t>
+          <t>manipulaca</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>2013</v>
+        <v>2150</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>nieprzyniósł</t>
+          <t>urzędowey</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Dominii nieprzyniósł kartki</t>
+          <t>manipulacyi urzędowey –</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>nieprzynieść</t>
+          <t>urzędowa</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>nieprzyniósł</t>
+          <t>urzędowey</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>nieprzyniósło</t>
+          <t>urzędowie</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>2121</v>
+        <v>2183</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ludowemi</t>
+          <t>Dziedzica</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>dziś ludowemi zwanych</t>
+          <t>od Dziedzica pensyę</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>ludowe</t>
+          <t>dziedzic</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>ludowemi</t>
+          <t>Dziedzic</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>ludowa</t>
+          <t>dziedzica</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>2149</v>
+        <v>2196</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>manipulacyi</t>
+          <t>ordynaryi</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>– manipulacyi urzędowey</t>
+          <t>korcy ordynaryi –</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>manipulacya</t>
+          <t>ordynarya</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>manipulacyi</t>
+          <t>ordynaryi</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>manipulaca</t>
+          <t>ordynary</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>2150</v>
+        <v>2211</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urzędowey</t>
+          <t>Dziedzica</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>manipulacyi urzędowey –</t>
+          <t>zastępował Dziedzica .</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>urzędowa</t>
+          <t>dziedzic</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>urzędowey</t>
+          <t>Dziedzic</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>urzędowie</t>
+          <t>dziedzica</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>2183</v>
+        <v>2215</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Dziedzica</t>
+          <t>szczupłey</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>od Dziedzica pensyę</t>
+          <t>tak szczupłey dotacyi</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>dziedzic</t>
+          <t>szczupła</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Dziedzic</t>
+          <t>szczupłey</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>dziedzica</t>
+          <t>szczupłea</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>2196</v>
+        <v>2216</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>ordynaryi</t>
+          <t>dotacyi</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>korcy ordynaryi –</t>
+          <t>szczupłey dotacyi uwzględniając</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>ordynarya</t>
+          <t>dotacya</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>ordynaryi</t>
+          <t>dotacyi</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>ordynary</t>
+          <t>dotacy</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>2211</v>
+        <v>2256</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Dziedzica</t>
+          <t>przytem</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>zastępował Dziedzica .</t>
+          <t>mając przytem jakiś</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>dziedzic</t>
+          <t>przyto</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Dziedzic</t>
+          <t>przytem</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>dziedzica</t>
+          <t>przyt</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>2215</v>
+        <v>2274</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>szczupłey</t>
+          <t>lepiey</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>tak szczupłey dotacyi</t>
+          <t>nieraz lepiey jak</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>szczupła</t>
+          <t>dobrze</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>szczupłey</t>
+          <t>lepiey</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>szczupłea</t>
+          <t>lepiey</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>2216</v>
+        <v>2298</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>dotacyi</t>
+          <t>ładąn</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>szczupłey dotacyi uwzględniając</t>
+          <t>– ładąn parą</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>dotacya</t>
+          <t>ładna</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>dotacyi</t>
+          <t>ładąn</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>dotacy</t>
+          <t>ładąn</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>2256</v>
+        <v>2328</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>przytem</t>
+          <t>Bludnikach</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>mając przytem jakiś</t>
+          <t>w Bludnikach –</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>przyto</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>przytem</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>przyt</t>
+          <t>Bludnik</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>2274</v>
+        <v>2331</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>lepiey</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>nieraz lepiey jak</t>
+          <t>do Bludnik należały</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>dobrze</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>lepiey</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>lepiey</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>2298</v>
+        <v>2335</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ładąn</t>
+          <t>Siedliska</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>– ładąn parą</t>
+          <t>i Siedliska –</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>ładna</t>
+          <t>Siedliska</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>ładąn</t>
+          <t>siedliski</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>ładąn</t>
+          <t>siedliska</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>2328</v>
+        <v>2340</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Bludnikach</t>
+          <t>Dziedzica</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>w Bludnikach –</t>
+          <t>nowego Dziedzica –</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>dziedzic</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>Dziedzic</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>dziedzica</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>2331</v>
+        <v>2403</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>zkończone</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>do Bludnik należały</t>
+          <t>białą zkończone )</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>zkończyć</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>zkończone</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>zkończone</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>2335</v>
+        <v>2415</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Siedliska</t>
+          <t>niewiem</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>i Siedliska –</t>
+          <t>– niewiem czy</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Siedliska</t>
+          <t>niewiem</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>siedliski</t>
+          <t>Niewiem</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>siedliska</t>
+          <t>niew</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>2340</v>
+        <v>2450</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Dziedzica</t>
+          <t>człowiecze</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>nowego Dziedzica –</t>
+          <t>Ty człowiecze na</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>dziedzic</t>
+          <t>człowiek</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Dziedzic</t>
+          <t>człowieczy</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>dziedzica</t>
+          <t>człowiec</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>2403</v>
+        <v>2454</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>zkończone</t>
+          <t>nieporadzisz</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>białą zkończone )</t>
+          <t>mi nieporadzisz –</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>zkończyć</t>
+          <t>nieporadzić</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>zkończone</t>
+          <t>niePoradzisz</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>zkończone</t>
+          <t>nieporadzisz</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>2415</v>
+        <v>2508</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>niewiem</t>
+          <t>mojey</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>– niewiem czy</t>
+          <t>za mojey pamięci</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>niewiem</t>
+          <t>mój</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Niewiem</t>
+          <t>mojey</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>niew</t>
+          <t>mojenie</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>2450</v>
+        <v>2513</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>człowiecze</t>
+          <t>Bludnikach</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Ty człowiecze na</t>
+          <t>w Bludnikach .</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>człowiek</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>człowieczy</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>człowiec</t>
+          <t>Bludnik</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>2454</v>
+        <v>2564</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>nieporadzisz</t>
+          <t>późney</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>mi nieporadzisz –</t>
+          <t>tak późney dokupił</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>nieporadzić</t>
+          <t>późno</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>niePoradzisz</t>
+          <t>późney</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>nieporadzisz</t>
+          <t>późnoy</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>2508</v>
+        <v>2573</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>mojey</t>
+          <t>Dochorowie</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>za mojey pamięci</t>
+          <t>W Dochorowie osadził</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>mój</t>
+          <t>Dochorów</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>mojey</t>
+          <t>Dochorowie</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>mojenie</t>
+          <t>dochór</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>2513</v>
+        <v>2575</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Bludnikach</t>
+          <t>nayjstarszego</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>w Bludnikach .</t>
+          <t>osadził nayjstarszego syna</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>stary</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>nayjstarszego</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>niejstarszy</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>2564</v>
+        <v>2589</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>późney</t>
+          <t>Toje</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>tak późney dokupił</t>
+          <t>– Toje diło</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>późno</t>
+          <t>toje</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>późney</t>
+          <t>Toje</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>późnoy</t>
+          <t>tój</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>2573</v>
+        <v>2595</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Dochorowie</t>
+          <t>Mychayłowu</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>W Dochorowie osadził</t>
+          <t>mojomu Mychayłowu .</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Dochorów</t>
+          <t>mychayłowu</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Dochorowie</t>
+          <t>Mychayłowu</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>dochór</t>
+          <t>mychaył</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>2575</v>
+        <v>2597</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>nayjstarszego</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>osadził nayjstarszego syna</t>
+          <t>. Bludniki oddał</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>stary</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>nayjstarszego</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>niejstarszy</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>2589</v>
+        <v>2601</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Toje</t>
+          <t>iOycu</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>– Toje diło</t>
+          <t>Józefowi iOycu mojemu</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>toje</t>
+          <t>ioyciec</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Toje</t>
+          <t>iOycu</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>tój</t>
+          <t>jOyc</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>2595</v>
+        <v>2642</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Mychayłowu</t>
+          <t>Siemginowa</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>mojomu Mychayłowu .</t>
+          <t>do Siemginowa –</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>mychayłowu</t>
+          <t>Siemginów</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Mychayłowu</t>
+          <t>Siemginowa</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>mychaył</t>
+          <t>siemginowa</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>2597</v>
+        <v>2646</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>dośmierci</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>. Bludniki oddał</t>
+          <t>aż dośmierci Oyca</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>dośmierć</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>dośmierci</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>dośmiert</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>2601</v>
+        <v>2647</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>iOycu</t>
+          <t>Oyca</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Józefowi iOycu mojemu</t>
+          <t>dośmierci Oyca przy</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>ioyciec</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>iOycu</t>
+          <t>Oyca</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>jOyc</t>
+          <t>oyca</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>2642</v>
+        <v>2710</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Siemginowa</t>
+          <t>niewinem</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>do Siemginowa –</t>
+          <t>Lipa niewinem .</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Siemginów</t>
+          <t>niewiedzieć</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Siemginowa</t>
+          <t>Niewino</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>siemginowa</t>
+          <t>niewine</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>2646</v>
+        <v>2720</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>dośmierci</t>
+          <t>Bludnikami</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>aż dośmierci Oyca</t>
+          <t>z Bludnikami o</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>dośmierć</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>dośmierci</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>dośmiert</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>2647</v>
+        <v>2728</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Oyca</t>
+          <t>Temerowiec</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>dośmierci Oyca przy</t>
+          <t>z Temerowiec ,</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>oyciec</t>
+          <t>Temerowice</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Oyca</t>
+          <t>Temerowiec</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>temerowiec</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>2710</v>
+        <v>2751</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>niewinem</t>
+          <t>Oycem</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Lipa niewinem .</t>
+          <t>za Oycem doszedłszy</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>niewiedzieć</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Niewino</t>
+          <t>Oycem</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>niewine</t>
+          <t>oycie</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>2720</v>
+        <v>2764</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Bludnikami</t>
+          <t>sukcessyi</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>z Bludnikami o</t>
+          <t>prawem sukcessyi przeszedł</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>sukcessya</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>sukcessyi</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>sukcessyj</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>2728</v>
+        <v>2804</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Temerowiec</t>
+          <t>niebył</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>z Temerowiec ,</t>
+          <t>– niebył gospodarzem</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Temerowice</t>
+          <t>niebyć</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Temerowiec</t>
+          <t>Niebyła</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>temerowiec</t>
+          <t>niebył</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>2751</v>
+        <v>2806</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Oycem</t>
+          <t>więcey</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>za Oycem doszedłszy</t>
+          <t>gospodarzem więcey fantasta</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>oyciec</t>
+          <t>dużo</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Oycem</t>
+          <t>więcey</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>oycie</t>
+          <t>więcea</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>2764</v>
+        <v>2847</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>sukcessyi</t>
+          <t>gołey</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>prawem sukcessyi przeszedł</t>
+          <t>na gołey podłodze</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>sukcessya</t>
+          <t>goła</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>sukcessyi</t>
+          <t>gołey</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>sukcessyj</t>
+          <t>goło</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>2804</v>
+        <v>2865</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>niebył</t>
+          <t>niemogli</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>– niebył gospodarzem</t>
+          <t>ci niemogli długo</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>niebyć</t>
+          <t>niemóc</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Niebyła</t>
+          <t>niemogel</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>niebył</t>
+          <t>niemogli</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>2806</v>
+        <v>2893</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>więcey</t>
+          <t>obeyściu</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>gospodarzem więcey fantasta</t>
+          <t>na obeyściu niemożna</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>dużo</t>
+          <t>obeyście</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>więcey</t>
+          <t>obeyściu</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>więcea</t>
+          <t>obeyść</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>2847</v>
+        <v>2894</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>gołey</t>
+          <t>niemożna</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>na gołey podłodze</t>
+          <t>obeyściu niemożna było</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>goła</t>
+          <t>niemóc</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>gołey</t>
+          <t>niemożny</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>goło</t>
+          <t>niemożna</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>2865</v>
+        <v>2931</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>niemogli</t>
+          <t>Oyca</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>ci niemogli długo</t>
+          <t>mojego Oyca spadała</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>niemóc</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>niemogel</t>
+          <t>Oyca</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>niemogli</t>
+          <t>oyca</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>2893</v>
+        <v>2938</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>obeyściu</t>
+          <t>Treterowej</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>na obeyściu niemożna</t>
+          <t>rodzonym Treterowej i</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>obeyście</t>
+          <t>Treterowa</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>obeyściu</t>
+          <t>Treterowej</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>obeyść</t>
+          <t>treterowa</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>2894</v>
+        <v>2940</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>niemożna</t>
+          <t>Swieżaskiey</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>obeyściu niemożna było</t>
+          <t>i Swieżaskiey .</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>niemóc</t>
+          <t>Swieżaska</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>niemożny</t>
+          <t>Swieżaskiey</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>niemożna</t>
+          <t>swieżaskie</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>2931</v>
+        <v>2963</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Oyca</t>
+          <t>Stryiskim</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>mojego Oyca spadała</t>
+          <t>w Stryiskim w</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>oyciec</t>
+          <t>Stryiskie</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Oyca</t>
+          <t>Stryiskim</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>stryiski</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>2938</v>
+        <v>2967</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Treterowej</t>
+          <t>Kruszelnicę</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>rodzonym Treterowej i</t>
+          <t>czy Kruszelnicę –</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Treterowa</t>
+          <t>Kruszelnica</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Treterowej</t>
+          <t>Kruszelnicę</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>treterowa</t>
+          <t>kruszelnica</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>2940</v>
+        <v>2976</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Swieżaskiey</t>
+          <t>generacyi</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>i Swieżaskiey .</t>
+          <t>kilka generacyi na</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Swieżaska</t>
+          <t>generacya</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Swieżaskiey</t>
+          <t>generacyi</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>swieżaskie</t>
+          <t>generacyj</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>2963</v>
+        <v>2979</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Stryiskim</t>
+          <t>obeyściu</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>w Stryiskim w</t>
+          <t>jednem obeyściu było</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Stryiskie</t>
+          <t>obeyście</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Stryiskim</t>
+          <t>obeyściu</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>stryiski</t>
+          <t>obeyść</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>2967</v>
+        <v>2986</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Kruszelnicę</t>
+          <t>niemając</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>czy Kruszelnicę –</t>
+          <t>Panny niemając widoków</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Kruszelnica</t>
+          <t>niemieć</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Kruszelnicę</t>
+          <t>niemając</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>kruszelnica</t>
+          <t>niemający</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>2976</v>
+        <v>3017</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>generacyi</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>kilka generacyi na</t>
+          <t>sąsiedztwo Bludnik do</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>generacya</t>
+          <t>Bludniki</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>generacyi</t>
+          <t>Bludnik</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>generacyj</t>
+          <t>bludnik</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>2979</v>
+        <v>3050</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>obeyściu</t>
+          <t>Siemiginowie</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>jednem obeyściu było</t>
+          <t>na Siemiginowie już</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>obeyście</t>
+          <t>Siemiginów</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>obeyściu</t>
+          <t>Siemiginowie</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>obeyść</t>
+          <t>siemigin</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>2986</v>
+        <v>3085</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>niemając</t>
+          <t>niema</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Panny niemając widoków</t>
+          <t>że niema sukcessorów</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4471,430 +4471,340 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>niemając</t>
+          <t>niema</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>niemający</t>
+          <t>niemy</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>3017</v>
+        <v>3127</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>Kruszelnicy</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>sąsiedztwo Bludnik do</t>
+          <t>do Kruszelnicy o</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Bludniki</t>
+          <t>Kruszelnica</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Bludnik</t>
+          <t>Kruszelnicy</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>bludnik</t>
+          <t>kruszelnik</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>3050</v>
+        <v>3131</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Siemiginowie</t>
+          <t>odległey</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>na Siemiginowie już</t>
+          <t>mil odległey od</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Siemiginów</t>
+          <t>odległa</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Siemiginowie</t>
+          <t>odległey</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>siemigin</t>
+          <t>odległea</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>3085</v>
+        <v>3133</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>niema</t>
+          <t>Siemignowa</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>że niema sukcessorów</t>
+          <t>od Siemignowa –</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>niemieć</t>
+          <t>Siemignów</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>niema</t>
+          <t>Siemignowa</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>niemy</t>
+          <t>siemignowa</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>3127</v>
+        <v>3143</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Kruszelnicy</t>
+          <t>łania</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>do Kruszelnicy o</t>
+          <t>jak łania Panna</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Kruszelnica</t>
+          <t>łania</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Kruszelnicy</t>
+          <t>łani</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>kruszelnik</t>
+          <t>łanie</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>3131</v>
+        <v>3171</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>odległey</t>
+          <t>Siemiginowa</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>mil odległey od</t>
+          <t>sukcessorka Siemiginowa –</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>odległa</t>
+          <t>Siemiginów</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>odległey</t>
+          <t>Siemiginowa</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>odległea</t>
+          <t>siemiginowa</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>3133</v>
+        <v>3185</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Siemignowa</t>
+          <t>Nawaryi</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>od Siemignowa –</t>
+          <t>koło Nawaryi i</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Siemignów</t>
+          <t>Nawarya</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Siemignowa</t>
+          <t>Nawaryi</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>siemignowa</t>
+          <t>nawary</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>3143</v>
+        <v>3207</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>łania</t>
+          <t>ciepłey</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>jak łania Panna</t>
+          <t>ale ciepłey wdowy</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>łania</t>
+          <t>ciepły</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>łani</t>
+          <t>ciepłey</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>łanie</t>
+          <t>ciepło</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>3171</v>
+        <v>3216</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Siemiginowa</t>
+          <t>Szołayskiego</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>sukcessorka Siemiginowa –</t>
+          <t>pana Szołayskiego młodzika</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Siemiginów</t>
+          <t>Szołayski</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Siemiginowa</t>
+          <t>Szołayskiego</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>siemiginowa</t>
+          <t>szołayski</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>3185</v>
+        <v>3230</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Nawaryi</t>
+          <t>pożyciu</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>koło Nawaryi i</t>
+          <t>nim pożyciu –</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Nawarya</t>
+          <t>pożycie</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Nawaryi</t>
+          <t>pożyć</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>nawary</t>
+          <t>pożyć</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>3207</v>
+        <v>3267</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>ciepłey</t>
+          <t>Lesniowic</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>ale ciepłey wdowy</t>
+          <t>do Lesniowic przyległe</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>ciepły</t>
+          <t>Lesniowice</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>ciepłey</t>
+          <t>Lesniowic</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>ciepło</t>
+          <t>lesniowice</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>3216</v>
+        <v>3269</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Szołayskiego</t>
+          <t>Mosty</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>pana Szołayskiego młodzika</t>
+          <t>przyległe Mosty .</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Szołayski</t>
+          <t>Mosty</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Szołayskiego</t>
+          <t>Most</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
-        <is>
-          <t>szołayski</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>3230</v>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>pożyciu</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>nim pożyciu –</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>pożycie</t>
-        </is>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>pożyć</t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>pożyć</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>3267</v>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Lesniowic</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>do Lesniowic przyległe</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Lesniowice</t>
-        </is>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>Lesniowic</t>
-        </is>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>lesniowice</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>3269</v>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Mosty</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>przyległe Mosty .</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Mosty</t>
-        </is>
-      </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>Most</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
         <is>
           <t>most</t>
         </is>

</xml_diff>